<commit_message>
made program function-based. made few bug fixes:-     1. multiplication function fixed     2. division function fixed new features:-     exponent function now supported
</commit_message>
<xml_diff>
--- a/excel and python calculator/excelsheet.xlsx
+++ b/excel and python calculator/excelsheet.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,13 +24,33 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -45,9 +65,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +455,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -454,7 +484,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>output</t>
         </is>
@@ -462,15 +492,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>+</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -478,20 +508,140 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">--&gt; </t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>enter your equation in this row.</t>
         </is>
       </c>
     </row>
+    <row r="4" ht="23.25" customHeight="1" s="6">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>OPPERATORS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1" s="6">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1" s="6">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>x (case sensitive)</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>multiply</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n"/>
+    </row>
+    <row r="8" ht="18.75" customHeight="1" s="6">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>divide</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1" s="6">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>^</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>power</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n"/>
+    </row>
+    <row r="10" ht="18.75" customHeight="1" s="6">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>--&gt;</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>